<commit_message>
Added Duval Pentagons Algorithm
</commit_message>
<xml_diff>
--- a/Distribution/xDGA Sample.xlsx
+++ b/Distribution/xDGA Sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Hydrogen</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Duval Triangles</t>
+  </si>
+  <si>
+    <t>For OLTC</t>
+  </si>
+  <si>
+    <t>Duval Pentagons</t>
   </si>
 </sst>
 </file>
@@ -471,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V56"/>
+  <dimension ref="B2:V61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1385,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
     </row>
-    <row r="49" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -1401,7 +1407,7 @@
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
     </row>
-    <row r="50" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -1423,8 +1429,11 @@
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
     </row>
-    <row r="51" spans="3:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C52" s="6" t="str">
         <f>_xll.DUVALTRIANGLES_OLTC(C14)</f>
         <v xml:space="preserve">[ Title =&gt; Interpretation of Dissolved Gas Analysis as per Duval Triangles for On-Load Tap Changers (OLTC) ]_x000D_
@@ -1452,7 +1461,7 @@
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
     </row>
-    <row r="53" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -1474,7 +1483,7 @@
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
     </row>
-    <row r="54" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -1496,7 +1505,7 @@
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
     </row>
-    <row r="55" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -1518,7 +1527,7 @@
       <c r="U55" s="6"/>
       <c r="V55" s="6"/>
     </row>
-    <row r="56" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -1540,8 +1549,106 @@
       <c r="U56" s="6"/>
       <c r="V56" s="6"/>
     </row>
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="6" t="str">
+        <f>_xll.DUVALPENTAGONS(C14)</f>
+        <v xml:space="preserve">[ Title =&gt; Interpretation of Dissolved Gas Analysis as per Duval Pentagons (IEEE Electrical Insulation Magazine, Nov/Dec - Vol. 30, No. 6, pg. 9-12) ]_x000D_
+[ Duval Pentagon 1 =&gt; S =&gt; Stray gassing of Oil (&lt; 200 oC) ]_x000D_
+[ Duval Pentagon 2 =&gt; S =&gt; Stray gassing of Oil (&lt; 200 oC) ]_x000D_
+</v>
+      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+    </row>
+    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+    </row>
+    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="6"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="6"/>
+      <c r="V60" s="6"/>
+    </row>
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C58:V61"/>
     <mergeCell ref="C17:V45"/>
     <mergeCell ref="C14:V14"/>
     <mergeCell ref="C15:V15"/>

</xml_diff>

<commit_message>
Added Rogers Ratios algorithm
</commit_message>
<xml_diff>
--- a/Distribution/xDGA Sample.xlsx
+++ b/Distribution/xDGA Sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Hydrogen</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Duval Pentagons</t>
+  </si>
+  <si>
+    <t>Rogers Ratios</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V61"/>
+  <dimension ref="B2:V69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,8 +1649,174 @@
       <c r="U61" s="6"/>
       <c r="V61" s="6"/>
     </row>
+    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" s="6" t="str">
+        <f>_xll.ROGERSRATIOS(C14)</f>
+        <v xml:space="preserve">[ Title =&gt; Interpretation of Dissolved Gas Analysis as per Rogers Ratios as described in IEEE C57.104 ]_x000D_
+[ C2H2/C2H4 =&gt; 0.500 ]_x000D_
+[ CH4/H2 =&gt; 0.400 ]_x000D_
+[ C2H4/C2H6 =&gt; 2.000 ]_x000D_
+[ Rogers Ratio Failure Code =&gt; NA =&gt; Not Available ]_x000D_
+</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="6"/>
+      <c r="T63" s="6"/>
+      <c r="U63" s="6"/>
+      <c r="V63" s="6"/>
+    </row>
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+      <c r="V64" s="6"/>
+    </row>
+    <row r="65" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
+      <c r="U65" s="6"/>
+      <c r="V65" s="6"/>
+    </row>
+    <row r="66" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+      <c r="U66" s="6"/>
+      <c r="V66" s="6"/>
+    </row>
+    <row r="67" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
+      <c r="U67" s="6"/>
+      <c r="V67" s="6"/>
+    </row>
+    <row r="68" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="6"/>
+    </row>
+    <row r="69" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+      <c r="U69" s="6"/>
+      <c r="V69" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C63:V69"/>
     <mergeCell ref="C58:V61"/>
     <mergeCell ref="C17:V45"/>
     <mergeCell ref="C14:V14"/>

</xml_diff>

<commit_message>
Corrected some errors on the areas defining the Duval Pentagons
</commit_message>
<xml_diff>
--- a/Distribution/xDGA Sample.xlsx
+++ b/Distribution/xDGA Sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Excel\Oil Analysis Tools\xDGA\Distribution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\EngineersTools\ElectricalEngineering\Transformers\xDGA\Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="B2:V69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="C52" sqref="C52:V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>